<commit_message>
made few changes to framework and updated test cases
</commit_message>
<xml_diff>
--- a/Automation/TestData/Tumi.xlsx
+++ b/Automation/TestData/Tumi.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20736" windowHeight="8880"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="8880" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="PlaceOrder" sheetId="1" r:id="rId1"/>
+    <sheet name="Registration" sheetId="2" r:id="rId2"/>
+    <sheet name="Cart" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="72">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -196,18 +196,54 @@
   </si>
   <si>
     <t>2 Beaver Creek Rd</t>
+  </si>
+  <si>
+    <t>ConfirmPassword</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>NewRegistration</t>
+  </si>
+  <si>
+    <t>Tumi</t>
+  </si>
+  <si>
+    <t>Ecom</t>
+  </si>
+  <si>
+    <t>Tumi1301193945@gmai.com</t>
+  </si>
+  <si>
+    <t>ExistingAccount</t>
+  </si>
+  <si>
+    <t>TumiEcom@123</t>
+  </si>
+  <si>
+    <t>VerifyCart</t>
+  </si>
+  <si>
+    <t>ProductQ</t>
+  </si>
+  <si>
+    <t>skurry@coredatalabs.com</t>
+  </si>
+  <si>
+    <t>Sharvah@189</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="00000"/>
     <numFmt numFmtId="165" formatCode="00000000000"/>
     <numFmt numFmtId="166" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,7 +281,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -279,15 +315,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -296,7 +323,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -305,22 +332,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -382,7 +404,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -414,10 +436,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -449,7 +470,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -625,36 +645,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:X8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="33.109375" customWidth="1"/>
-    <col min="15" max="15" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.5546875" customWidth="1"/>
-    <col min="20" max="20" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -697,38 +723,38 @@
       <c r="N1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="U1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="V1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="W1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="X1" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -747,10 +773,20 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
       <c r="N2" s="2"/>
-      <c r="S2" s="11"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -776,7 +812,7 @@
       <c r="I3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="6" t="s">
         <v>26</v>
       </c>
       <c r="K3" s="4">
@@ -785,74 +821,89 @@
       <c r="L3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="13" t="s">
+      <c r="M3" s="8" t="s">
         <v>38</v>
       </c>
       <c r="N3" s="2">
         <v>123</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="2">
         <v>4</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="2">
         <v>2020</v>
       </c>
-      <c r="U3" t="s">
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2" t="s">
         <v>49</v>
       </c>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:24">
+      <c r="A4" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>47</v>
       </c>
+      <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="6">
         <v>7080</v>
       </c>
       <c r="K4" s="4">
         <v>12345678901</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="13" t="s">
+      <c r="M4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="2">
         <v>123</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="2">
         <v>6</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="2">
         <v>2020</v>
       </c>
-      <c r="U4" t="s">
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:24">
+      <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -861,10 +912,30 @@
       <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="10"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:24">
+      <c r="A6" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -873,158 +944,155 @@
       <c r="C6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="K6">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2">
         <v>5555555555</v>
       </c>
-      <c r="M6" s="12"/>
-      <c r="Q6" t="s">
+      <c r="L6" s="2"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:24">
+      <c r="A7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D7" t="s">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H7" t="s">
+      <c r="G7" s="2"/>
+      <c r="H7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="2">
         <v>17301</v>
       </c>
-      <c r="K7" s="14">
+      <c r="K7" s="11">
         <v>2345678901</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M7" s="15" t="s">
+      <c r="M7" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="2">
         <v>1234</v>
       </c>
-      <c r="O7" s="10">
+      <c r="O7" s="7">
         <v>3</v>
       </c>
-      <c r="P7" s="10">
+      <c r="P7" s="7">
         <v>2019</v>
       </c>
-      <c r="R7">
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2">
         <v>1</v>
       </c>
-      <c r="S7">
+      <c r="S7" s="2">
         <v>2</v>
       </c>
-      <c r="T7">
+      <c r="T7" s="2">
         <v>3</v>
       </c>
-      <c r="U7" t="s">
+      <c r="U7" s="2" t="s">
         <v>51</v>
       </c>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="8" spans="1:24">
+      <c r="A8" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D8" t="s">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="H8" t="s">
+      <c r="G8" s="2"/>
+      <c r="H8" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="2">
         <v>17301</v>
       </c>
-      <c r="K8" s="14">
+      <c r="K8" s="11">
         <v>2345678901</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M8" s="15" t="s">
+      <c r="M8" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="2">
         <v>1234</v>
       </c>
-      <c r="O8" s="10">
+      <c r="O8" s="7">
         <v>3</v>
       </c>
-      <c r="P8" s="10">
+      <c r="P8" s="7">
         <v>2019</v>
       </c>
-      <c r="U8" t="s">
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="V8" t="s">
+      <c r="V8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="W8" t="s">
+      <c r="W8" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="X8" t="s">
+      <c r="X8" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="M9" s="10"/>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="M11" s="10"/>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="M12" s="10"/>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="M13" s="10"/>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="M14" s="10"/>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="M15" s="10"/>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="M16" s="10"/>
-    </row>
-    <row r="17" spans="13:13" x14ac:dyDescent="0.3">
-      <c r="M17" s="10"/>
-    </row>
-    <row r="18" spans="13:13" x14ac:dyDescent="0.3">
-      <c r="M18" s="10"/>
-    </row>
-    <row r="19" spans="13:13" x14ac:dyDescent="0.3">
-      <c r="M19" s="10"/>
-    </row>
-    <row r="20" spans="13:13" x14ac:dyDescent="0.3">
-      <c r="M20" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1040,25 +1108,139 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Working on new functions
</commit_message>
<xml_diff>
--- a/Automation/TestData/Tumi.xlsx
+++ b/Automation/TestData/Tumi.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="8880"/>
@@ -337,13 +337,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="00000"/>
     <numFmt numFmtId="165" formatCode="00000000000"/>
     <numFmt numFmtId="166" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -438,7 +438,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -476,9 +476,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -540,7 +538,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -572,10 +570,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -607,7 +604,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -783,14 +779,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AA14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="AA13" sqref="AA13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="27.85546875" customWidth="1"/>
     <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
@@ -821,7 +817,7 @@
     <col min="27" max="27" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -904,7 +900,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -937,8 +933,9 @@
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AA2" s="2"/>
+    </row>
+    <row r="3" spans="1:27">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -997,8 +994,9 @@
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AA3" s="2"/>
+    </row>
+    <row r="4" spans="1:27">
       <c r="A4" s="2" t="s">
         <v>31</v>
       </c>
@@ -1057,8 +1055,9 @@
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AA4" s="2"/>
+    </row>
+    <row r="5" spans="1:27">
       <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
@@ -1091,8 +1090,9 @@
       <c r="X5" s="2"/>
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AA5" s="2"/>
+    </row>
+    <row r="6" spans="1:27">
       <c r="A6" s="2" t="s">
         <v>32</v>
       </c>
@@ -1129,8 +1129,9 @@
       <c r="X6" s="2"/>
       <c r="Y6" s="2"/>
       <c r="Z6" s="2"/>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AA6" s="2"/>
+    </row>
+    <row r="7" spans="1:27">
       <c r="A7" s="2" t="s">
         <v>39</v>
       </c>
@@ -1193,8 +1194,9 @@
       <c r="X7" s="2"/>
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AA7" s="2"/>
+    </row>
+    <row r="8" spans="1:27">
       <c r="A8" s="2" t="s">
         <v>52</v>
       </c>
@@ -1257,8 +1259,9 @@
         <v>58</v>
       </c>
       <c r="Z8" s="2"/>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AA8" s="2"/>
+    </row>
+    <row r="9" spans="1:27">
       <c r="A9" s="2" t="s">
         <v>72</v>
       </c>
@@ -1317,8 +1320,9 @@
       <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AA9" s="2"/>
+    </row>
+    <row r="10" spans="1:27">
       <c r="A10" s="2" t="s">
         <v>75</v>
       </c>
@@ -1349,8 +1353,9 @@
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AA10" s="2"/>
+    </row>
+    <row r="11" spans="1:27">
       <c r="A11" s="2" t="s">
         <v>77</v>
       </c>
@@ -1385,8 +1390,9 @@
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
       <c r="Z11" s="2"/>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AA11" s="2"/>
+    </row>
+    <row r="12" spans="1:27">
       <c r="A12" s="2" t="s">
         <v>95</v>
       </c>
@@ -1447,23 +1453,27 @@
       <c r="Z12" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A13" s="23" t="s">
+      <c r="AA12" s="2"/>
+    </row>
+    <row r="13" spans="1:27">
+      <c r="A13" s="10" t="s">
         <v>99</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>47</v>
       </c>
+      <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="23" t="s">
+      <c r="F13" s="10" t="s">
         <v>100</v>
       </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
       <c r="I13" s="2" t="s">
         <v>89</v>
       </c>
@@ -1473,7 +1483,7 @@
       <c r="K13" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="2">
         <v>9087654400</v>
       </c>
       <c r="M13" s="2" t="s">
@@ -1485,38 +1495,48 @@
       <c r="O13" s="2">
         <v>123</v>
       </c>
-      <c r="P13" s="24">
+      <c r="P13" s="23">
         <v>10</v>
       </c>
-      <c r="Q13" s="24">
+      <c r="Q13" s="23">
         <v>2028</v>
       </c>
-      <c r="V13" s="23" t="s">
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="10" t="s">
         <v>49</v>
       </c>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
       <c r="Z13" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="AA13" t="s">
+      <c r="AA13" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:27">
+      <c r="A14" s="2" t="s">
         <v>102</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="C14" s="2"/>
+      <c r="D14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="E14" s="10" t="s">
         <v>11</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
       <c r="I14" s="2" t="s">
         <v>44</v>
       </c>
@@ -1526,7 +1546,7 @@
       <c r="K14" s="2">
         <v>17301</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="2">
         <v>9087654400</v>
       </c>
       <c r="M14" s="2" t="s">
@@ -1538,22 +1558,26 @@
       <c r="O14" s="2">
         <v>1234</v>
       </c>
-      <c r="P14" s="24">
+      <c r="P14" s="23">
         <v>12</v>
       </c>
-      <c r="Q14" s="24">
+      <c r="Q14" s="23">
         <v>2028</v>
       </c>
-      <c r="V14" s="23" t="s">
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="AA14" t="s">
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2"/>
+      <c r="AA14" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="AA16" s="1"/>
-      <c r="AB16" s="25"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1574,14 +1598,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
@@ -1604,7 +1628,7 @@
     <col min="26" max="26" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1684,7 +1708,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26">
       <c r="A2" s="21" t="s">
         <v>96</v>
       </c>
@@ -1718,7 +1742,7 @@
       <c r="Y2" s="21"/>
       <c r="Z2" s="21"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1733,7 +1757,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26">
       <c r="A4" t="s">
         <v>81</v>
       </c>
@@ -1745,7 +1769,7 @@
       </c>
       <c r="N4" s="14"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26">
       <c r="A5" t="s">
         <v>84</v>
       </c>
@@ -1757,7 +1781,7 @@
       </c>
       <c r="N5" s="14"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26">
       <c r="A6" t="s">
         <v>87</v>
       </c>
@@ -1769,7 +1793,7 @@
       </c>
       <c r="N6" s="14"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26">
       <c r="A7" t="s">
         <v>88</v>
       </c>
@@ -1822,7 +1846,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" ht="15.75" thickBot="1">
       <c r="A8" t="s">
         <v>91</v>
       </c>
@@ -1875,7 +1899,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" ht="15.75" thickBot="1">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -1912,14 +1936,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
@@ -1930,7 +1954,7 @@
     <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1953,7 +1977,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -1973,7 +1997,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>66</v>
       </c>
@@ -1991,14 +2015,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
@@ -2006,7 +2030,7 @@
     <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2023,7 +2047,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>68</v>
       </c>

</xml_diff>

<commit_message>
working framework enchancements and test cases
</commit_message>
<xml_diff>
--- a/Automation/TestData/Tumi.xlsx
+++ b/Automation/TestData/Tumi.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FA5956-56D7-4BFB-A388-0222D940770A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20736" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="8880"/>
   </bookViews>
   <sheets>
     <sheet name="PlaceOrder" sheetId="1" r:id="rId1"/>
@@ -194,9 +193,6 @@
     <t>test2</t>
   </si>
   <si>
-    <t>Hi….</t>
-  </si>
-  <si>
     <t>ConfirmPassword</t>
   </si>
   <si>
@@ -360,18 +356,21 @@
   </si>
   <si>
     <t>tag</t>
+  </si>
+  <si>
+    <t>Hi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="00000"/>
     <numFmt numFmtId="165" formatCode="00000000000"/>
     <numFmt numFmtId="166" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -704,7 +703,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -736,27 +735,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -788,24 +769,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -981,45 +944,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AA22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="Y19" sqref="Y19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.89453125" customWidth="1"/>
-    <col min="2" max="2" width="26.41796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.41796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1015625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.68359375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5234375" customWidth="1"/>
-    <col min="8" max="8" width="12.89453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5234375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.68359375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.41796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.89453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.3125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.41796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.41796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="6" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="15" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.68359375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.68359375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.89453125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.5234375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.89453125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.68359375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="25.3125" customWidth="1"/>
+    <col min="23" max="23" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:27">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1039,7 +1002,7 @@
         <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>13</v>
@@ -1096,13 +1059,13 @@
         <v>55</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1137,7 +1100,7 @@
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:27">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1198,7 +1161,7 @@
       <c r="Z3" s="2"/>
       <c r="AA3" s="2"/>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:27">
       <c r="A4" s="2" t="s">
         <v>31</v>
       </c>
@@ -1259,7 +1222,7 @@
       <c r="Z4" s="2"/>
       <c r="AA4" s="2"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:27">
       <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
@@ -1294,7 +1257,7 @@
       <c r="Z5" s="2"/>
       <c r="AA5" s="2"/>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:27">
       <c r="A6" s="2" t="s">
         <v>32</v>
       </c>
@@ -1333,7 +1296,7 @@
       <c r="Z6" s="2"/>
       <c r="AA6" s="2"/>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:27">
       <c r="A7" s="2" t="s">
         <v>39</v>
       </c>
@@ -1398,7 +1361,7 @@
       <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:27">
       <c r="A8" s="2" t="s">
         <v>52</v>
       </c>
@@ -1458,14 +1421,14 @@
         <v>57</v>
       </c>
       <c r="Y8" s="2" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
       <c r="Z8" s="2"/>
       <c r="AA8" s="2"/>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:27">
       <c r="A9" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>7</v>
@@ -1478,7 +1441,7 @@
         <v>11</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="10" t="s">
@@ -1488,10 +1451,10 @@
         <v>25</v>
       </c>
       <c r="J9" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K9" s="13" t="s">
         <v>103</v>
-      </c>
-      <c r="K9" s="13" t="s">
-        <v>104</v>
       </c>
       <c r="L9" s="4">
         <v>12345678902</v>
@@ -1524,9 +1487,9 @@
       <c r="Z9" s="2"/>
       <c r="AA9" s="2"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:27">
       <c r="A10" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>7</v>
@@ -1539,7 +1502,7 @@
         <v>11</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -1547,10 +1510,10 @@
         <v>25</v>
       </c>
       <c r="J10" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K10" s="13" t="s">
         <v>103</v>
-      </c>
-      <c r="K10" s="13" t="s">
-        <v>104</v>
       </c>
       <c r="L10" s="4">
         <v>12345678902</v>
@@ -1589,9 +1552,9 @@
       <c r="Z10" s="2"/>
       <c r="AA10" s="2"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:27">
       <c r="A11" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>7</v>
@@ -1604,7 +1567,7 @@
         <v>11</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -1612,10 +1575,10 @@
         <v>25</v>
       </c>
       <c r="J11" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K11" s="13" t="s">
         <v>103</v>
-      </c>
-      <c r="K11" s="13" t="s">
-        <v>104</v>
       </c>
       <c r="L11" s="4">
         <v>12345678902</v>
@@ -1649,14 +1612,14 @@
         <v>57</v>
       </c>
       <c r="Y11" s="2" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
       <c r="Z11" s="2"/>
       <c r="AA11" s="2"/>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:27">
       <c r="A12" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1679,7 +1642,7 @@
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
       <c r="V12" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W12" s="2"/>
       <c r="X12" s="2"/>
@@ -1687,15 +1650,15 @@
       <c r="Z12" s="2"/>
       <c r="AA12" s="2"/>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:27">
       <c r="A13" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -1724,9 +1687,9 @@
       <c r="Z13" s="2"/>
       <c r="AA13" s="2"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:27">
       <c r="A14" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>7</v>
@@ -1748,13 +1711,13 @@
         <v>43</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K14" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L14" s="4">
         <v>12345678901</v>
@@ -1783,13 +1746,13 @@
       <c r="X14" s="2"/>
       <c r="Y14" s="2"/>
       <c r="Z14" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AA14" s="2"/>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:27">
       <c r="A15" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>47</v>
@@ -1802,18 +1765,18 @@
         <v>11</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>16</v>
       </c>
       <c r="K15" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L15" s="2">
         <v>9087654400</v>
@@ -1844,15 +1807,15 @@
       <c r="X15" s="2"/>
       <c r="Y15" s="2"/>
       <c r="Z15" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AA15" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27">
       <c r="A16" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>47</v>
@@ -1901,19 +1864,19 @@
       <c r="T16" s="2"/>
       <c r="U16" s="2"/>
       <c r="V16" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="W16" s="2"/>
       <c r="X16" s="2"/>
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
       <c r="AA16" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27">
       <c r="A17" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>7</v>
@@ -1964,7 +1927,7 @@
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
       <c r="V17" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="W17" s="2"/>
       <c r="X17" s="2"/>
@@ -1972,9 +1935,9 @@
       <c r="Z17" s="2"/>
       <c r="AA17" s="2"/>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:27">
       <c r="A18" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>7</v>
@@ -2029,7 +1992,7 @@
         <v>3</v>
       </c>
       <c r="V18" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="W18" s="2"/>
       <c r="X18" s="2"/>
@@ -2037,9 +2000,9 @@
       <c r="Z18" s="2"/>
       <c r="AA18" s="2"/>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:27">
       <c r="A19" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>7</v>
@@ -2088,7 +2051,7 @@
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
       <c r="V19" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="W19" s="2" t="s">
         <v>56</v>
@@ -2097,16 +2060,16 @@
         <v>57</v>
       </c>
       <c r="Y19" s="2" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
       <c r="Z19" s="2"/>
       <c r="AA19" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27">
       <c r="A20" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>7</v>
@@ -2155,27 +2118,27 @@
       <c r="T20" s="2"/>
       <c r="U20" s="2"/>
       <c r="V20" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="W20" s="2"/>
       <c r="X20" s="2"/>
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
       <c r="AA20" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27">
       <c r="A21" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z21" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27">
+      <c r="A22" t="s">
         <v>111</v>
-      </c>
-      <c r="Z21" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" t="s">
-        <v>112</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>7</v>
@@ -2227,24 +2190,24 @@
       <c r="X22" s="2"/>
       <c r="Y22" s="2"/>
       <c r="Z22" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AA22" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B3" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B9" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B13" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B14" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B15" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B16" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B4" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="B17" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="B22" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B5" r:id="rId2"/>
+    <hyperlink ref="B6" r:id="rId3"/>
+    <hyperlink ref="B3" r:id="rId4"/>
+    <hyperlink ref="B9" r:id="rId5"/>
+    <hyperlink ref="B13" r:id="rId6"/>
+    <hyperlink ref="B14" r:id="rId7"/>
+    <hyperlink ref="B15" r:id="rId8"/>
+    <hyperlink ref="B16" r:id="rId9"/>
+    <hyperlink ref="B4" r:id="rId10"/>
+    <hyperlink ref="B17" r:id="rId11"/>
+    <hyperlink ref="B22" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="360" r:id="rId13"/>
@@ -2252,37 +2215,37 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:Z9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.68359375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.68359375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.89453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.68359375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1015625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5234375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.3125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.3125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.1015625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.89453125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.68359375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.3125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="17" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.1015625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.89453125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.68359375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:26">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -2302,7 +2265,7 @@
         <v>12</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H1" s="18" t="s">
         <v>13</v>
@@ -2359,18 +2322,18 @@
         <v>55</v>
       </c>
       <c r="Z1" s="20" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26">
       <c r="A2" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="C2" s="22" t="s">
         <v>94</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>95</v>
       </c>
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
@@ -2396,7 +2359,7 @@
       <c r="Y2" s="22"/>
       <c r="Z2" s="23"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:26">
       <c r="A3" s="21" t="s">
         <v>28</v>
       </c>
@@ -2429,18 +2392,18 @@
       <c r="X3" s="22"/>
       <c r="Y3" s="22"/>
       <c r="Z3" s="23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26">
+      <c r="A4" s="21" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="21" t="s">
+      <c r="B4" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="C4" s="22" t="s">
         <v>79</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>80</v>
       </c>
       <c r="D4" s="22"/>
       <c r="E4" s="22"/>
@@ -2466,15 +2429,15 @@
       <c r="Y4" s="22"/>
       <c r="Z4" s="23"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:26">
       <c r="A5" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="C5" s="22" t="s">
         <v>82</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>83</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
@@ -2500,12 +2463,12 @@
       <c r="Y5" s="22"/>
       <c r="Z5" s="23"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:26">
       <c r="A6" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C6" s="22">
         <v>123</v>
@@ -2534,9 +2497,9 @@
       <c r="Y6" s="22"/>
       <c r="Z6" s="23"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:26">
       <c r="A7" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>4</v>
@@ -2558,13 +2521,13 @@
       </c>
       <c r="H7" s="22"/>
       <c r="I7" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J7" s="22" t="s">
         <v>16</v>
       </c>
       <c r="K7" s="26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L7" s="4">
         <v>12345678901</v>
@@ -2593,15 +2556,15 @@
       <c r="X7" s="22"/>
       <c r="Y7" s="22"/>
       <c r="Z7" s="23" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="15.75" thickBot="1">
       <c r="A8" s="21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>5</v>
@@ -2620,13 +2583,13 @@
       </c>
       <c r="H8" s="22"/>
       <c r="I8" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J8" s="22" t="s">
         <v>16</v>
       </c>
       <c r="K8" s="26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L8" s="4">
         <v>12345678901</v>
@@ -2655,15 +2618,15 @@
       <c r="X8" s="22"/>
       <c r="Y8" s="22"/>
       <c r="Z8" s="23" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="15.75" thickBot="1">
       <c r="A9" s="28" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C9" s="30" t="s">
         <v>29</v>
@@ -2694,37 +2657,37 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="B7" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="B8" r:id="rId4" display="Employee.tumi@gmail.com" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="B9" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="B2" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2"/>
+    <hyperlink ref="B7" r:id="rId3"/>
+    <hyperlink ref="B8" r:id="rId4" display="Employee.tumi@gmail.com"/>
+    <hyperlink ref="B9" r:id="rId5"/>
+    <hyperlink ref="B2" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.41796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1015625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.68359375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1015625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.68359375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.41796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2735,7 +2698,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>8</v>
@@ -2744,63 +2707,63 @@
         <v>10</v>
       </c>
       <c r="G1" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>61</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" t="s">
         <v>62</v>
       </c>
-      <c r="C2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F2" t="s">
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.3125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5234375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.1015625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.89453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2814,21 +2777,21 @@
         <v>2</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" t="s">
         <v>69</v>
-      </c>
-      <c r="D2" t="s">
-        <v>70</v>
       </c>
       <c r="E2">
         <v>5</v>
@@ -2836,8 +2799,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>